<commit_message>
Remove all non numeric characters from tel number
</commit_message>
<xml_diff>
--- a/Customers1.xlsx
+++ b/Customers1.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="79">
   <si>
     <t xml:space="preserve">firstname</t>
   </si>
@@ -53,148 +53,157 @@
     <t xml:space="preserve">Anja</t>
   </si>
   <si>
+    <t xml:space="preserve">+46731264413</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test2_firstname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test2_lastname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malmö</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gogo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0046731212345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test3_firstname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test3_lastname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gothenburg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+4673123-4412</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test4_firstname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test4_lastname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ivan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">004673 123-3332</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test5_firstname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test5_lastname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nynäshamn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">076 111 12 34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test6_firstname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test6_lastname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">75 113 1244</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test7_firstname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test7_lastname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08 444 555</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test8_firstname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test8_lastname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">085556666</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test9_firstname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test9_lastname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08-123-1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test10_firstname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test10_lastname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tiva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08555-6666</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test1_firstname1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test1_lastname1</t>
+  </si>
+  <si>
     <t xml:space="preserve">+46731264412</t>
   </si>
   <si>
-    <t xml:space="preserve">test2_firstname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test2_lastname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Malmö</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gogo</t>
+    <t xml:space="preserve">test2_firstname2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test2_lastname2</t>
   </si>
   <si>
     <t xml:space="preserve">0046731235412</t>
   </si>
   <si>
-    <t xml:space="preserve">test3_firstname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test3_lastname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gothenburg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+4673123-4412</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test4_firstname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test4_lastname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ivan</t>
+    <t xml:space="preserve">test3_firstname3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test3_lastname3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test4_firstname4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test4_lastname4</t>
   </si>
   <si>
     <t xml:space="preserve">004673 123-4412</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test5_firstname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test5_lastname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nynäshamn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">076 111 12 34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test6_firstname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test6_lastname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coko</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75 113 1244</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test7_firstname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test7_lastname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moko</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08 444 555</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test8_firstname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test8_lastname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Loko</t>
-  </si>
-  <si>
-    <t xml:space="preserve">085556666</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test9_firstname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test9_lastname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08-123-1234</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test10_firstname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test10_lastname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tiva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08555-6666</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test1_firstname1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test1_lastname1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test2_firstname2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test2_lastname2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test3_firstname3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test3_lastname3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test4_firstname4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test4_lastname4</t>
   </si>
   <si>
     <t xml:space="preserve">test5_firstname5</t>
@@ -353,7 +362,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -649,7 +658,7 @@
         <v>51</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>18</v>
@@ -657,13 +666,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>13</v>
@@ -671,10 +680,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>20</v>
@@ -685,13 +694,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>8</v>
@@ -699,10 +708,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>29</v>
@@ -713,10 +722,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
@@ -727,10 +736,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>37</v>
@@ -741,10 +750,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>41</v>
@@ -755,10 +764,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>45</v>
@@ -769,10 +778,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>49</v>
@@ -783,13 +792,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>8</v>
@@ -797,13 +806,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
remove first chat if it is a space (" ").
</commit_message>
<xml_diff>
--- a/Customers1.xlsx
+++ b/Customers1.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="81">
   <si>
     <t xml:space="preserve">firstname</t>
   </si>
@@ -53,7 +53,7 @@
     <t xml:space="preserve">Anja</t>
   </si>
   <si>
-    <t xml:space="preserve">+46731264413</t>
+    <t xml:space="preserve"> +46731264413</t>
   </si>
   <si>
     <t xml:space="preserve">test2_firstname</t>
@@ -68,7 +68,7 @@
     <t xml:space="preserve">Gogo</t>
   </si>
   <si>
-    <t xml:space="preserve">0046731212345</t>
+    <t xml:space="preserve"> 0046731212345</t>
   </si>
   <si>
     <t xml:space="preserve">test3_firstname</t>
@@ -146,94 +146,100 @@
     <t xml:space="preserve">Loko</t>
   </si>
   <si>
+    <t xml:space="preserve"> 085556666</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test9_firstname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test9_lastname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 08-123-1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test10_firstname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test10_lastname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tiva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08555-6666</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test1_firstname1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test1_lastname1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+46731264412</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test2_firstname2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test2_lastname2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0046731235412</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test3_firstname3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test3_lastname3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test4_firstname4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test4_lastname4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">004673 123-4412</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test5_firstname5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test5_lastname5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test6_firstname6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test6_lastname6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test7_firstname7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test7_lastname7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test8_firstname8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test8_lastname8</t>
+  </si>
+  <si>
     <t xml:space="preserve">085556666</t>
   </si>
   <si>
-    <t xml:space="preserve">test9_firstname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test9_lastname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mo</t>
+    <t xml:space="preserve">test9_firstname9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test9_lastname9</t>
   </si>
   <si>
     <t xml:space="preserve">08-123-1234</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test10_firstname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test10_lastname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tiva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08555-6666</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test1_firstname1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test1_lastname1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+46731264412</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test2_firstname2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test2_lastname2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0046731235412</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test3_firstname3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test3_lastname3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test4_firstname4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test4_lastname4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">004673 123-4412</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test5_firstname5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test5_lastname5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test6_firstname6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test6_lastname6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test7_firstname7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test7_lastname7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test8_firstname8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test8_lastname8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test9_firstname9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test9_lastname9</t>
   </si>
   <si>
     <t xml:space="preserve">test10_firstname10</t>
@@ -362,7 +368,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -756,7 +762,7 @@
         <v>68</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>18</v>
@@ -764,13 +770,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>8</v>
@@ -778,10 +784,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>49</v>
@@ -792,13 +798,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>8</v>
@@ -806,13 +812,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>8</v>

</xml_diff>